<commit_message>
Rough Code Changes incl. Doc Changes
</commit_message>
<xml_diff>
--- a/doc/crypto-janeczek-mair-working-hours.xlsx
+++ b/doc/crypto-janeczek-mair-working-hours.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Janeczek" sheetId="8" r:id="rId1"/>
@@ -12,17 +12,17 @@
     <sheet name="SUM" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="SumActJaneczek">Janeczek!$F$8</definedName>
-    <definedName name="SumActMair">Mair!$F$9</definedName>
-    <definedName name="SumEstJaneczek">Janeczek!$E$8</definedName>
-    <definedName name="SumEstMair">Mair!$E$9</definedName>
+    <definedName name="SumActJaneczek">Janeczek!$F$9</definedName>
+    <definedName name="SumActMair">Mair!$F$10</definedName>
+    <definedName name="SumEstJaneczek">Janeczek!$E$9</definedName>
+    <definedName name="SumEstMair">Mair!$E$10</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>PHASE</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Erstellung erster Verschlüsselungsmethoden</t>
+  </si>
+  <si>
+    <t>Learning from examples</t>
+  </si>
+  <si>
+    <t>trying to get back into the code</t>
   </si>
 </sst>
 </file>
@@ -180,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -203,13 +209,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF31859C"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF31859C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF31859C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF31859C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF31859C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF31859C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF31859C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF31859C"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -268,14 +311,23 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -649,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -675,14 +727,14 @@
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1"/>
@@ -776,30 +828,43 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="28.15" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="14">
-        <f>SUM(E5:E7)</f>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="F8" s="14">
-        <f>SUM(F5:F7)</f>
-        <v>7.9166666666666663E-2</v>
-      </c>
-      <c r="G8" s="4"/>
+      <c r="B8" s="19">
+        <v>42047</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F8" s="17">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="B9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="14">
+        <f>SUM(E5:E8)</f>
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F9" s="14">
+        <f>SUM(F5:F8)</f>
+        <v>0.12083333333333332</v>
+      </c>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1"/>
@@ -825,9 +890,17 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -837,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G9"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -854,14 +927,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2"/>
@@ -956,7 +1029,7 @@
       <c r="C8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="18">
@@ -968,25 +1041,45 @@
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19">
+        <v>42047</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F9" s="17">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="14">
-        <f>SUM(E5:E8)</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="F9" s="14">
-        <f>SUM(F4:F8)</f>
-        <v>0.19444444444444445</v>
-      </c>
-      <c r="G9" s="4"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="14">
+        <f>SUM(E5:E9)</f>
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="F10" s="14">
+        <f>SUM(F4:F9)</f>
+        <v>0.2361111111111111</v>
+      </c>
+      <c r="G10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -996,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:D8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1007,12 +1100,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:4" ht="18.75">
       <c r="B4" s="5"/>
@@ -1035,11 +1128,11 @@
       </c>
       <c r="C6" s="15">
         <f>SumEstJaneczek</f>
-        <v>0.33333333333333337</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D6" s="16">
         <f>SumActJaneczek</f>
-        <v>7.9166666666666663E-2</v>
+        <v>0.12083333333333332</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1048,11 +1141,11 @@
       </c>
       <c r="C7" s="15">
         <f>SumEstMair</f>
-        <v>0.22222222222222221</v>
+        <v>0.24305555555555555</v>
       </c>
       <c r="D7" s="16">
         <f>SumActMair</f>
-        <v>0.19444444444444445</v>
+        <v>0.2361111111111111</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1061,11 +1154,11 @@
       </c>
       <c r="C8" s="15">
         <f>SUM(SumEstJaneczek+SumEstMair)</f>
-        <v>0.55555555555555558</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="D8" s="16">
         <f>SUM(SumActJaneczek+SumActMair)</f>
-        <v>0.27361111111111114</v>
+        <v>0.3569444444444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>